<commit_message>
- Indicateur de complétude des données de calcul de l'ouvrage - MAJ Excel (forumules)
</commit_message>
<xml_diff>
--- a/EIEx/EIEx/Données/Etude test.xlsx
+++ b/EIEx/EIEx/Données/Etude test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="290" windowWidth="15480" windowHeight="11640" tabRatio="811" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="290" windowWidth="15480" windowHeight="11640" tabRatio="811" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PG" sheetId="32" r:id="rId1"/>
@@ -3835,7 +3835,7 @@
     <sheetView showZeros="0" view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A11" sqref="A11"/>
-      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5"/>
@@ -13263,10 +13263,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W394"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView showFormulas="1" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="C11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5"/>
@@ -31057,10 +31057,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W192"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView showZeros="0" view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J1:J1048576"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5"/>

</xml_diff>